<commit_message>
feat-update the pipeline according to comments
</commit_message>
<xml_diff>
--- a/ComplementaryData/TargetProtein.xlsx
+++ b/ComplementaryData/TargetProtein.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feiranl/Documents/GitHub/pcSecYeast/ComplementaryData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12D6AB-C908-A34B-98B3-590D6437EF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14307C-006A-F049-8702-1E712A3DA1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protein_info" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="144">
   <si>
     <t>Length</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>fake protein to validate the FSEOF result</t>
+  </si>
+  <si>
+    <t>glucosidase</t>
+  </si>
+  <si>
+    <t>MRFPSIFTAVLFAASSALAAPVNTTTEDETAQIPAEAVIGYSDLEGDFDVAVLPFSNSTNNGLLFINTTIASIAAKEEGVSLDKREEGEPKASIPSSASVQLDSYNYDGSTFSGKIYVKNIAYSKKVTVIYADGSDNWNNNGNTIAASYSAPISGSNYEYWTFSASINGIKEFYIKYEVSGKTYYDNNNSANYQVSTSKPTTTTATATTTTAPSTSTTTPPSRSEPATFPTGNSTISSWIKKQEGISRFAMLRNINPPGSATGFIAASLSTAGPDYYYAWTRDAALTSNVIVYEYNTTLSGNKTILNVLKDYVTFSVKTQSTSTVCNCLGEPKFNPDASGYTGAWGRPQNDGPAERATTFILFADSYLTQTKDASYVTGTLKPAIFKDLDYVVNVWSNGCFDLWEEVNGVHFYTLMVMRKGLLLGADFAKRNGDSTRASTYSSTASTIANKISSFWVSSNNWIQVSQSVTGGVSKKGLDVSTLLAANLGSVDDGFFTPGSEKILATAVAVEDSFASLYPINKNLPSYLGNSIGRYPEDTYNGNGNSQGNSWFLAVTGYAELYYRAIKEWIGNGGVTVSSISLPFFKKFDSSATSGKKYTVGTSDFNNLAQNIALAADRFLSTVQLHAHNNGSLAEEFDRTTGLSTGARDLTWSHASLITASYAKAGAPAA</t>
   </si>
 </sst>
 </file>
@@ -1354,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457B43B4-2D2D-1B46-BFA5-ABA224C89B8B}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3180,6 +3186,50 @@
         <v>42</v>
       </c>
     </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>5</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L42" s="1">
+        <v>670</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N42" s="1">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="2" priority="10"/>

</xml_diff>

<commit_message>
update the code for some bugs
</commit_message>
<xml_diff>
--- a/ComplementaryData/TargetProtein.xlsx
+++ b/ComplementaryData/TargetProtein.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10313"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feiranl/Documents/GitHub/pcSecYeast/ComplementaryData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC14307C-006A-F049-8702-1E712A3DA1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A7C37F-5888-0F4B-AC4C-E2A9BADA3A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="145">
   <si>
     <t>Length</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>MRFPSIFTAVLFAASSALAAPVNTTTEDETAQIPAEAVIGYSDLEGDFDVAVLPFSNSTNNGLLFINTTIASIAAKEEGVSLDKREEGEPKASIPSSASVQLDSYNYDGSTFSGKIYVKNIAYSKKVTVIYADGSDNWNNNGNTIAASYSAPISGSNYEYWTFSASINGIKEFYIKYEVSGKTYYDNNNSANYQVSTSKPTTTTATATTTTAPSTSTTTPPSRSEPATFPTGNSTISSWIKKQEGISRFAMLRNINPPGSATGFIAASLSTAGPDYYYAWTRDAALTSNVIVYEYNTTLSGNKTILNVLKDYVTFSVKTQSTSTVCNCLGEPKFNPDASGYTGAWGRPQNDGPAERATTFILFADSYLTQTKDASYVTGTLKPAIFKDLDYVVNVWSNGCFDLWEEVNGVHFYTLMVMRKGLLLGADFAKRNGDSTRASTYSSTASTIANKISSFWVSSNNWIQVSQSVTGGVSKKGLDVSTLLAANLGSVDDGFFTPGSEKILATAVAVEDSFASLYPINKNLPSYLGNSIGRYPEDTYNGNGNSQGNSWFLAVTGYAELYYRAIKEWIGNGGVTVSSISLPFFKKFDSSATSGKKYTVGTSDFNNLAQNIALAADRFLSTVQLHAHNNGSLAEEFDRTTGLSTGARDLTWSHASLITASYAKAGAPAA</t>
+  </si>
+  <si>
+    <t>AmylasePost</t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457B43B4-2D2D-1B46-BFA5-ABA224C89B8B}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2895,7 +2898,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -2924,7 +2927,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>81</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>24</v>
       </c>
@@ -2982,7 +2985,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>2351</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>86</v>
       </c>
@@ -3142,7 +3145,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
@@ -3228,6 +3231,59 @@
       </c>
       <c r="N42" s="1">
         <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L43" s="2">
+        <v>569</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N43" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="S43" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>